<commit_message>
bento local find ddn selection script working
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_LocalSearch.xlsx
+++ b/InputFiles/TC01_Bento_LocalSearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7C14D6-4B45-4C9A-93D7-BDD5DC640F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53208C8A-AAB2-4864-B0D2-F95A4F93E030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -116,23 +116,29 @@
 	samp.sample_id AS `Sample ID`</t>
   </si>
   <si>
-    <t>MATCH (ss:study_subject)
-  WHERE ss.study_subject_id = 'BENTO-CASE-3405467'
-MATCH (ss)-[:study_subject_of_study]-&gt;(s:study)-[:study_of_program]-&gt;(p)
-OPTIONAL MATCH (ss)&lt;-[*..2]-(parent)&lt;--(f:file)
-OPTIONAL MATCH (f)-[:file_of_laboratory_procedure]-&gt;(lp)
-RETURN
-  COUNT(DISTINCT ss) AS study_subjects,
-  COUNT(DISTINCT s) AS studies,
-  COUNT(DISTINCT p) AS programs,
-  COUNT(DISTINCT f) AS files,
-  COUNT(DISTINCT lp) AS assays</t>
-  </si>
-  <si>
     <t>SamplesTab</t>
   </si>
   <si>
     <t>FilesTab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+WHERE ss.study_subject_id = 'BENTO-CASE-3405467'
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
+MATCH (samp)&lt;-[:file_of_sample]-(f)
+MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
+RETURN COUNT(DISTINCT p) AS Programs,
+COUNT(DISTINCT s) AS Arms,
+COUNT(DISTINCT ss) AS Cases,
+COUNT(DISTINCT samp) AS Samples,
+COUNT(DISTINCT lp) AS Assays,
+COUNT(DISTINCT f) AS Files
+</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -553,13 +559,13 @@
     </row>
     <row r="3" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -568,15 +574,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>

</xml_diff>